<commit_message>
Updating documents for iteration 2
</commit_message>
<xml_diff>
--- a/docs/CS673Team1_weeklyreport.xlsx
+++ b/docs/CS673Team1_weeklyreport.xlsx
@@ -9,6 +9,7 @@
     <sheet state="visible" name="Mike Eskowitz" sheetId="4" r:id="rId6"/>
     <sheet state="visible" name="Cory Stone" sheetId="5" r:id="rId7"/>
     <sheet state="visible" name="Ed Orsini" sheetId="6" r:id="rId8"/>
+    <sheet state="visible" name="Ravi K.Rajendran" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="134">
   <si>
     <t>week #
  (from date - end date)</t>
@@ -89,78 +90,30 @@
     <t>4 (2/9/ - 2/15)</t>
   </si>
   <si>
-    <t>5 (2/17 - 2/23)</t>
+    <t xml:space="preserve"> 0 - research MEAN Stack</t>
   </si>
   <si>
-    <t>0-learning angular js and node.js</t>
-  </si>
-  <si>
-    <t>6 (2/24 - 3/2)</t>
-  </si>
-  <si>
-    <t>3- wokring for about me page using bootstrap
-3.workinf on designing of authorization page.</t>
-  </si>
-  <si>
-    <t>7 (3/3 - 3/9)</t>
-  </si>
-  <si>
-    <t>0- learning animation and dynamic page chnages</t>
-  </si>
-  <si>
-    <t>8 (3/10 - 3/16)</t>
-  </si>
-  <si>
-    <t>3.designingauthorization page</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0 - research MEAN Stack</t>
+    <t>5 (2/17 - 2/23)</t>
   </si>
   <si>
     <t xml:space="preserve">
 3- start project</t>
   </si>
   <si>
-    <t xml:space="preserve">2-begin designing db models schema and cloud environment
-3-more coding
-</t>
-  </si>
-  <si>
-    <t>3-adding to existing project code,
- implementing web-socket into backend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">research 
-chat
-deployment research
-universal socket factory for the front end of the application
-chat socket configuration
-</t>
-  </si>
-  <si>
-    <t>chat 
-deployment research, async js research, websockket research
-Angular and node JS Security</t>
-  </si>
-  <si>
-    <t>merge
-chat room front end design
-chat front end controller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Socket Event handler
-instant messaging databse object controller
-private chat
-started working on a user search algorithm
-</t>
-  </si>
-  <si>
     <t>0 - read tutorials on Node.js 
 and MongoDB</t>
   </si>
   <si>
+    <t>0-learning angular js and node.js</t>
+  </si>
+  <si>
     <t>0 - look through sample project
 code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-begin designing db models schema and cloud environment
+3-more coding
+</t>
   </si>
   <si>
     <t>0,2</t>
@@ -175,6 +128,10 @@
     <t>2,3</t>
   </si>
   <si>
+    <t>3-adding to existing project code,
+ implementing web-socket into backend</t>
+  </si>
+  <si>
     <t>2 - decide on how the posts  
 should look on the wall
 3 - start writing html code for the posts</t>
@@ -183,8 +140,22 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
+    <t>6 (2/24 - 3/2)</t>
+  </si>
+  <si>
     <t>3 - start writing back end
 functionality for wall posts</t>
+  </si>
+  <si>
+    <t>7 (3/3 - 3/9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">research 
+chat
+deployment research
+universal socket factory for the front end of the application
+chat socket configuration
+</t>
   </si>
   <si>
     <t>3 - add finishing touches to wall
@@ -196,9 +167,69 @@
     <t>3,2</t>
   </si>
   <si>
+    <t>8 (3/10 - 3/16)</t>
+  </si>
+  <si>
+    <t>3- wokring for about me page using bootstrap
+3.workinf on designing of authorization page.</t>
+  </si>
+  <si>
+    <t>chat 
+deployment research, async js research, websockket research
+Angular and node JS Security</t>
+  </si>
+  <si>
     <t>2 - start looking into how to add
 comments to a post
 3 - work on defect</t>
+  </si>
+  <si>
+    <t>0- learning animation and dynamic page chnages</t>
+  </si>
+  <si>
+    <t>merge
+chat room front end design
+chat front end controller</t>
+  </si>
+  <si>
+    <t>9 (3/17 - 3/23)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Socket Event handler
+instant messaging databse object controller
+private chat
+started working on a user search algorithm
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Added users stories to backlog 1 - Backlog grooming and iteration planning with team 3 - start initial coding for Comments </t>
+  </si>
+  <si>
+    <t>3.designingauthorization page</t>
+  </si>
+  <si>
+    <t>10 (3/24 - 3/30)</t>
+  </si>
+  <si>
+    <t>3 - Add functionality to send a friend Request</t>
+  </si>
+  <si>
+    <t>0-Learning angular js for chat feature</t>
+  </si>
+  <si>
+    <t>Teaching team about angular</t>
+  </si>
+  <si>
+    <t>11 (3/31 - 4/6)</t>
+  </si>
+  <si>
+    <t>Teaching sub group about anuglar/socketio</t>
+  </si>
+  <si>
+    <t>3 - add functionality to accept friend request and add friend and deny request 5. Meet to plan for presentation and prepare for demo</t>
+  </si>
+  <si>
+    <t>3,1</t>
   </si>
   <si>
     <t>1 (1/19/2017 - 1/25/2017)</t>
@@ -226,48 +257,6 @@
   </si>
   <si>
     <t>0 - read up on node.js</t>
-  </si>
-  <si>
-    <t>5 (2/16/2017 - 2/22/2017)</t>
-  </si>
-  <si>
-    <t>3 - worked on implementing profile options page in the application</t>
-  </si>
-  <si>
-    <t>Implement profile options page</t>
-  </si>
-  <si>
-    <t>6 (2/23/2017 - 3/1/2017)</t>
-  </si>
-  <si>
-    <t>3 - wored on implementing profile options page in the application</t>
-  </si>
-  <si>
-    <t>Finish implementation of profile options page</t>
-  </si>
-  <si>
-    <t>7 (3/2/2017 - 3/8/2017)</t>
-  </si>
-  <si>
-    <t>3 - Integrated profile feature with development branch</t>
-  </si>
-  <si>
-    <t>Work on presentation and paper</t>
-  </si>
-  <si>
-    <t>5 - Prepared slides for the presentation</t>
-  </si>
-  <si>
-    <t>8 (3/9/2017 - 3/15/2017)</t>
-  </si>
-  <si>
-    <t>3 - Reviews integration changes to get profile to work</t>
-  </si>
-  <si>
-    <t>Begin new feature development</t>
-  </si>
-  <si>
-    <t>5 - Editted slides and reviewed paper</t>
   </si>
   <si>
     <t>0 - Reading tutorials, setting up environment, and doing traning exercises for MEAN technology stack
@@ -298,13 +287,22 @@
 1 - Investigating capabilities of node modules to do OAuth with Facebook/Google</t>
   </si>
   <si>
+    <t>5 (2/16/2017 - 2/22/2017)</t>
+  </si>
+  <si>
     <t>0 - Continue learning about node.js
 1 - Finish Requirements section of SPPP
 1 - Finish SQAP section of SPPP
 2 - Work on design for authentication</t>
   </si>
   <si>
+    <t>3 - worked on implementing profile options page in the application</t>
+  </si>
+  <si>
     <t>4 (2/10 - 2/16)</t>
+  </si>
+  <si>
+    <t>Implement profile options page</t>
   </si>
   <si>
     <t>0 - Learning about express.js
@@ -314,10 +312,19 @@
 5 - Coordinate with team on SPPP and presentation</t>
   </si>
   <si>
+    <t>6 (2/23/2017 - 3/1/2017)</t>
+  </si>
+  <si>
     <t>0 - Continue learning about node and express.js
 1 - Create some user stories for authentication
 2 - Work on design for authentication
 3 - Start implementation for authentication</t>
+  </si>
+  <si>
+    <t>3 - wored on implementing profile options page in the application</t>
+  </si>
+  <si>
+    <t>Finish implementation of profile options page</t>
   </si>
   <si>
     <t>0 - Learning about express.js
@@ -325,9 +332,18 @@
 3 - Implementing Facebook OAuth</t>
   </si>
   <si>
+    <t>7 (3/2/2017 - 3/8/2017)</t>
+  </si>
+  <si>
     <t>0 - Continue learning about express.js
 1 - Create user stories for OAuth with Facebook, Google
 3 - Add unit tests for Authentication modules, give detailed description for team members to follow</t>
+  </si>
+  <si>
+    <t>3 - Integrated profile feature with development branch</t>
+  </si>
+  <si>
+    <t>Work on presentation and paper</t>
   </si>
   <si>
     <t>0 - Learning about express.js
@@ -341,20 +357,97 @@
 4 - Start preparing test plan</t>
   </si>
   <si>
+    <t>5 - Prepared slides for the presentation</t>
+  </si>
+  <si>
     <t>1 - Added users stories to backlog
 3 - Worked with team to merge everyone's work
 4 - Created test plan
 4 - Tested features</t>
   </si>
   <si>
+    <t>8 (3/9/2017 - 3/15/2017)</t>
+  </si>
+  <si>
     <t>3 - Implement Google OAuth
 4 - Finish all testing for iteration 1</t>
+  </si>
+  <si>
+    <t>3 - Reviews integration changes to get profile to work</t>
+  </si>
+  <si>
+    <t>Begin new feature development</t>
   </si>
   <si>
     <t>3 - Added more unit tests
 3 - Implemented Google OAuth
 4 - Tested items in test plan
 4 - Bug fixes</t>
+  </si>
+  <si>
+    <t>5 - Editted slides and reviewed paper</t>
+  </si>
+  <si>
+    <t>1 - Add user stories to backlog
+1 - Backlog grooming and prioritization
+3 - Work on combining profile data and wall posts into single view</t>
+  </si>
+  <si>
+    <t>9 (3/16/2017 - 3/22/2017)</t>
+  </si>
+  <si>
+    <t>1 - Added users stories to backlog
+1 - Backlog grooming and iteration planning with team
+3 - Combined the user's profile data and wall posts into a single view</t>
+  </si>
+  <si>
+    <t>3 - attempted to merge profile info and wall pages</t>
+  </si>
+  <si>
+    <t>3 - Allow users to view other users' profiles
+3 - Don't show other users' profiles as editable forms</t>
+  </si>
+  <si>
+    <t>Attempt to get backend to produce other user's profile pages</t>
+  </si>
+  <si>
+    <t>10 (3/23/2017 - 3/29/2017)</t>
+  </si>
+  <si>
+    <t>3 - Allow users to view other users' profile pages
+3 - Add toggle option for making profile info form editable</t>
+  </si>
+  <si>
+    <t>Bad week.  Didn't have time to do anything so far.</t>
+  </si>
+  <si>
+    <t>3 - Don't show other users' profiles as editable forms
+3 - Only show wall posts for the profile you are viewing
+4 - Update test plan and run regression tests
+4 - Collect test results for testing report, include code coverage</t>
+  </si>
+  <si>
+    <t>11 (3/30/2017 - 4/5/2017)</t>
+  </si>
+  <si>
+    <t>0 - Read through documentation regarding route script file</t>
+  </si>
+  <si>
+    <t>3 - Make wall posts specific to a user, a user's wall posts appear only on their profile
+3 - When logged in, navigation link to profile page will add user's id to the url so the correct profile is shown
+3 - Users can only edit their own profile
+3 - Help with implementation of friends/friend requests
+4 - Updated test plan
+4 - Tested features</t>
+  </si>
+  <si>
+    <t>3 - modified routing code to support passing of profile data by performing an http get on api/profile/username</t>
+  </si>
+  <si>
+    <t>4 - performed iteration 2 regression testing</t>
+  </si>
+  <si>
+    <t>12 (4/6/2017 - 4/12/2017)</t>
   </si>
   <si>
     <t>0 - Learning more about the MEAN stack via tutorials.
@@ -375,18 +468,75 @@
 5 - Caught up on slack messages.</t>
   </si>
   <si>
+    <t>0 - started learning about how to upload files using Express
+3 - installed Multer module and learned how to use it
+3 - worked with team to merge all feature branches to development branch</t>
+  </si>
+  <si>
     <t>7 (3/3 - 3-9)</t>
   </si>
   <si>
+    <t>3 - worked with team to merge all feature branches to development branch</t>
+  </si>
+  <si>
     <t>0 - watched video posted by Professor regarding Juice
-6 - working on content for presentation of iteration 1</t>
+6 - working on content for presentation of iteration 1 (with Mike)
+6 - worked on design document</t>
+  </si>
+  <si>
+    <t>3 - merged feature branches to development branch
+3 - worked on "friends" feature - created view and displayed user's friends
+4 - testing development branch after merging
+6 - met with entire team in order to enter stories for iteration #2, prioritized them, and set up teams to work on them</t>
+  </si>
+  <si>
+    <t>3 - working on deleting a friend
+4 - working on unit testing for picture feature and for friends feature</t>
+  </si>
+  <si>
+    <t>1 - cleaned up user stories to refine requirements and user acceptance tests
+3 - worked with team to integrate `request friend` button on wall
+4 - worked with team to remove hardcoded references to specific users (that was done while developing/testing)
+4 - tested and accepted stories and Pivotal Tracker 
+6 - met with team to iron out plan for presentation/demo of Iteration #2
+6 - started the slides for Iteration #2 demo</t>
+  </si>
+  <si>
+    <t>0- Learning MEAN basics</t>
+  </si>
+  <si>
+    <t>0- MEAN Tutorials
+5- Webex Meeting with team</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>0- Mongo and Node tutorials 
+2- Realtime webRTC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-Express tutorials
+3- Implemented a simple chat feature </t>
+  </si>
+  <si>
+    <t>0- Angular tutorials
+6- Implemented a server-client data transfer</t>
+  </si>
+  <si>
+    <t>0-Angular directives
+3- Implementing one-to-one chatting</t>
+  </si>
+  <si>
+    <t>2- Chat design
+3- Implementing chat scroll feature</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -398,6 +548,10 @@
     <font/>
     <font>
       <color rgb="FFFF0000"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <name val="Arial"/>
@@ -428,7 +582,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -440,20 +594,32 @@
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -463,27 +629,31 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
-<file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
-<file path=xl/drawings/worksheetdrawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
-<file path=xl/drawings/worksheetdrawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
-<file path=xl/drawings/worksheetdrawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
-<file path=xl/drawings/worksheetdrawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -701,7 +871,7 @@
     </row>
     <row r="6" ht="34.5" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3">
         <v>5.0</v>
@@ -713,7 +883,7 @@
         <v>1.0</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F6" s="3">
         <v>3.0</v>
@@ -731,7 +901,7 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B7" s="3">
         <v>4.0</v>
@@ -743,7 +913,7 @@
         <v>1.0</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="F7" s="3">
         <v>2.0</v>
@@ -761,7 +931,7 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B8" s="3">
         <v>4.0</v>
@@ -773,7 +943,7 @@
         <v>2.0</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="G8" s="3">
         <v>1.0</v>
@@ -791,13 +961,19 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>40</v>
+      </c>
+      <c r="B9" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>5.0</v>
       </c>
       <c r="D9" s="3">
         <v>0.5</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="I9" s="3">
         <v>4.5</v>
@@ -807,12 +983,24 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="C10" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="3">
+        <v>3.0</v>
+      </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -834,10 +1022,18 @@
       <c r="Z10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="A11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="C11" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2.0</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -15032,7 +15228,7 @@
         <v>1.0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="F2" s="3">
         <v>5.0</v>
@@ -15052,7 +15248,7 @@
         <v>2.0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F3" s="3"/>
       <c r="I3" s="3">
@@ -15073,7 +15269,7 @@
         <v>2.0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F4" s="3"/>
       <c r="H4" s="3">
@@ -15097,7 +15293,7 @@
         <v>2.0</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="3"/>
       <c r="I5" s="3">
@@ -15106,7 +15302,7 @@
     </row>
     <row r="6" ht="58.5" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3">
         <v>7.0</v>
@@ -15118,12 +15314,12 @@
         <v>1.0</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" ht="39.0" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B7" s="3">
         <v>8.0</v>
@@ -15135,12 +15331,12 @@
         <v>1.0</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" ht="36.0" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B8" s="3">
         <v>10.0</v>
@@ -15152,12 +15348,12 @@
         <v>2.0</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" ht="29.25" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B9" s="3">
         <v>9.0</v>
@@ -15169,7 +15365,58 @@
         <v>1.0</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>36</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="C10" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="C11" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="C12" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -15246,7 +15493,7 @@
         <v>1.0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="F2" s="3">
         <v>6.0</v>
@@ -15269,7 +15516,7 @@
         <v>2.0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F3" s="3">
         <v>5.0</v>
@@ -15292,13 +15539,13 @@
         <v>2.0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="F4" s="3">
         <v>5.0</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="N4" s="3">
         <v>8.0</v>
@@ -15315,7 +15562,7 @@
         <v>2.0</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="F5" s="3">
         <v>2.0</v>
@@ -15324,7 +15571,7 @@
         <v>4.0</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="N5" s="3">
         <v>10.0</v>
@@ -15332,7 +15579,7 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3">
         <v>7.0</v>
@@ -15341,10 +15588,10 @@
         <v>1.0</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="H6" s="3">
         <v>1.0</v>
@@ -15361,7 +15608,7 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B7" s="3">
         <v>9.0</v>
@@ -15370,7 +15617,7 @@
         <v>1.0</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="I7" s="3">
         <v>8.0</v>
@@ -15384,7 +15631,7 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B8" s="3">
         <v>9.0</v>
@@ -15393,7 +15640,7 @@
         <v>2.0</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I8" s="3">
         <v>5.0</v>
@@ -15405,7 +15652,7 @@
         <v>2.0</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="N8" s="3">
         <v>8.0</v>
@@ -15413,7 +15660,7 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B9" s="3">
         <v>4.0</v>
@@ -15422,7 +15669,7 @@
         <v>1.0</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H9" s="3">
         <v>2.0</v>
@@ -15435,7 +15682,90 @@
       </c>
     </row>
     <row r="10">
-      <c r="D10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="I10" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="K10" s="3"/>
+      <c r="M10" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="N10" s="3">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="C11" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="K11" s="3"/>
+      <c r="M11" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="N11" s="3">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="3">
+        <v>9.0</v>
+      </c>
+      <c r="C12" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="K12" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N12" s="3">
+        <v>8.0</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -15449,7 +15779,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.0"/>
+    <col customWidth="1" min="1" max="1" width="23.14"/>
     <col customWidth="1" min="2" max="2" width="33.14"/>
     <col customWidth="1" min="3" max="3" width="22.0"/>
     <col customWidth="1" min="4" max="4" width="16.29"/>
@@ -15518,7 +15848,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B2" s="3">
         <v>6.0</v>
@@ -15530,7 +15860,7 @@
         <v>1.0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="F2" s="3">
         <v>5.0</v>
@@ -15569,7 +15899,7 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B3" s="3">
         <v>5.0</v>
@@ -15581,7 +15911,7 @@
         <v>1.0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="F3" s="3">
         <v>4.0</v>
@@ -15601,7 +15931,7 @@
       <c r="K3" s="3">
         <v>0.0</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="6">
         <v>0.0</v>
       </c>
       <c r="M3" s="3"/>
@@ -15622,7 +15952,7 @@
     </row>
     <row r="4" ht="16.5" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B4" s="3">
         <v>8.0</v>
@@ -15634,7 +15964,7 @@
         <v>1.0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="F4" s="3">
         <v>1.0</v>
@@ -15679,7 +16009,7 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -15704,7 +16034,7 @@
     </row>
     <row r="6" ht="4.5" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B6" s="3">
         <v>8.0</v>
@@ -15716,7 +16046,7 @@
         <v>1.0</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="F6" s="3">
         <v>1.0</v>
@@ -15756,22 +16086,22 @@
       <c r="Y6" s="2"/>
     </row>
     <row r="7" ht="19.5" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="7">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="8">
         <v>8.0</v>
       </c>
       <c r="O7" s="2"/>
@@ -15788,7 +16118,7 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="B8" s="3">
         <v>8.0</v>
@@ -15800,7 +16130,7 @@
         <v>1.0</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="F8" s="3">
         <v>0.0</v>
@@ -15824,7 +16154,7 @@
         <v>0.0</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="N8" s="3">
         <v>8.0</v>
@@ -15843,7 +16173,7 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="B9" s="3">
         <v>5.0</v>
@@ -15855,7 +16185,7 @@
         <v>1.0</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="F9" s="3">
         <v>0.0</v>
@@ -15879,7 +16209,7 @@
         <v>0.0</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="N9" s="3">
         <v>8.0</v>
@@ -15898,7 +16228,7 @@
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="B10" s="3">
         <v>12.0</v>
@@ -15910,7 +16240,7 @@
         <v>4.0</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="F10" s="3">
         <v>1.0</v>
@@ -15934,7 +16264,7 @@
         <v>0.0</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="N10" s="3">
         <v>8.0</v>
@@ -15957,7 +16287,7 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -15981,7 +16311,7 @@
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="B12" s="3">
         <v>9.0</v>
@@ -15993,7 +16323,7 @@
         <v>4.0</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="F12" s="3">
         <v>0.0</v>
@@ -16017,7 +16347,7 @@
         <v>0.0</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="N12" s="3">
         <v>8.0</v>
@@ -16035,12 +16365,8 @@
       <c r="Y12" s="2"/>
     </row>
     <row r="13">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -16062,19 +16388,48 @@
       <c r="Y13" s="2"/>
     </row>
     <row r="14">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
+      <c r="A14" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="C14" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="K14" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="L14" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="N14" s="3">
+        <v>8.0</v>
+      </c>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
@@ -16088,13 +16443,48 @@
       <c r="Y14" s="2"/>
     </row>
     <row r="15">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
+      <c r="A15" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="K15" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="L15" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="N15" s="3">
+        <v>8.0</v>
+      </c>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
@@ -16108,20 +16498,46 @@
       <c r="Y15" s="2"/>
     </row>
     <row r="16">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="4"/>
+      <c r="A16" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B16" s="3">
+        <v>18.0</v>
+      </c>
+      <c r="C16" s="3">
+        <v>16.0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F16" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I16" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="J16" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="K16" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="L16" s="6">
+        <v>0.0</v>
+      </c>
       <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
+      <c r="N16" s="3">
+        <v>8.0</v>
+      </c>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
@@ -16137,7 +16553,9 @@
     <row r="17">
       <c r="A17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>111</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -16159,7 +16577,9 @@
     <row r="18">
       <c r="A18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
@@ -16173,7 +16593,9 @@
       <c r="Y18" s="2"/>
     </row>
     <row r="19">
-      <c r="A19" s="3"/>
+      <c r="A19" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="G19" s="3"/>
@@ -29180,7 +29602,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
@@ -29188,7 +29613,7 @@
     <col customWidth="1" min="2" max="2" width="32.57"/>
     <col customWidth="1" min="3" max="3" width="21.86"/>
     <col customWidth="1" min="4" max="4" width="16.14"/>
-    <col customWidth="1" min="5" max="5" width="27.86"/>
+    <col customWidth="1" min="5" max="5" width="26.0"/>
     <col customWidth="1" min="6" max="12" width="17.71"/>
     <col customWidth="1" min="13" max="13" width="25.86"/>
     <col customWidth="1" min="14" max="14" width="17.71"/>
@@ -29263,7 +29688,7 @@
         <v>1.0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F2" s="3">
         <v>4.5</v>
@@ -29272,7 +29697,7 @@
         <v>0.5</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="N2" s="3">
         <v>8.0</v>
@@ -29292,7 +29717,7 @@
         <v>2.0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F3" s="3">
         <v>2.0</v>
@@ -29301,7 +29726,7 @@
         <v>1.0</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="N3" s="3">
         <v>6.0</v>
@@ -29309,7 +29734,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B4" s="3">
         <v>5.0</v>
@@ -29321,7 +29746,7 @@
         <v>1.0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F4" s="3">
         <v>3.0</v>
@@ -29330,7 +29755,7 @@
         <v>1.0</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="N4" s="3">
         <v>6.0</v>
@@ -29338,7 +29763,7 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B5" s="3">
         <v>8.0</v>
@@ -29350,7 +29775,7 @@
         <v>1.0</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F5" s="3">
         <v>3.0</v>
@@ -29370,7 +29795,7 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3">
         <v>8.0</v>
@@ -29382,7 +29807,7 @@
         <v>1.0</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F6" s="3">
         <v>3.0</v>
@@ -29394,7 +29819,7 @@
         <v>3.0</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="N6" s="3">
         <v>6.0</v>
@@ -29402,7 +29827,7 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B7" s="3">
         <v>9.0</v>
@@ -29414,7 +29839,7 @@
         <v>1.0</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F7" s="3">
         <v>2.0</v>
@@ -29426,7 +29851,7 @@
         <v>3.0</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="N7" s="3">
         <v>8.0</v>
@@ -29434,7 +29859,7 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B8" s="3">
         <v>9.0</v>
@@ -29446,7 +29871,7 @@
         <v>2.0</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="G8" s="3">
         <v>1.0</v>
@@ -29458,7 +29883,7 @@
         <v>3.0</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="N8" s="3">
         <v>4.0</v>
@@ -29466,7 +29891,7 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B9" s="3">
         <v>7.0</v>
@@ -29478,12 +29903,105 @@
         <v>1.5</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="I9" s="3">
         <v>4.5</v>
       </c>
       <c r="J9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="N9" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="C10" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="D10" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G10" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="I10" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="N10" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="C11" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="I11" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="N11" s="3">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="3">
+        <v>14.5</v>
+      </c>
+      <c r="C12" s="3">
+        <v>13.5</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="I12" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="J12" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="K12" s="3">
         <v>1.0</v>
       </c>
     </row>
@@ -29580,7 +30098,7 @@
         <v>1.0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="F2" s="3">
         <v>6.0</v>
@@ -29619,7 +30137,7 @@
         <v>2.5</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="F3" s="3">
         <v>2.0</v>
@@ -29646,7 +30164,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B4" s="3">
         <v>6.0</v>
@@ -29658,7 +30176,7 @@
         <v>1.0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="F4" s="3">
         <v>4.0</v>
@@ -29686,7 +30204,7 @@
     </row>
     <row r="5" ht="27.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="B5" s="3">
         <v>2.5</v>
@@ -29696,7 +30214,7 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3">
@@ -29724,7 +30242,7 @@
     </row>
     <row r="6" ht="34.5" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3">
         <v>6.0</v>
@@ -29734,7 +30252,7 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="F6" s="3">
         <v>3.0</v>
@@ -29763,7 +30281,7 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B7" s="3">
         <v>15.0</v>
@@ -29774,7 +30292,9 @@
       <c r="D7" s="3">
         <v>2.0</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="F7" s="3">
         <v>4.0</v>
       </c>
@@ -29802,7 +30322,7 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="B8" s="3">
         <v>8.0</v>
@@ -29813,7 +30333,9 @@
       <c r="D8" s="3">
         <v>6.0</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -29840,7 +30362,7 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B9" s="3">
         <v>16.0</v>
@@ -29852,7 +30374,7 @@
         <v>4.0</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>94</v>
+        <v>122</v>
       </c>
       <c r="F9" s="3">
         <v>1.0</v>
@@ -29879,17 +30401,38 @@
       <c r="Y9" s="2"/>
     </row>
     <row r="10">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="C10" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1.0</v>
+      </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="I10" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="L10" s="3">
+        <v>3.0</v>
+      </c>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="2"/>
@@ -29905,16 +30448,33 @@
       <c r="Y10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="A11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="C11" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>124</v>
+      </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="K11" s="3"/>
+      <c r="I11" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0.5</v>
+      </c>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="2"/>
@@ -29930,17 +30490,33 @@
       <c r="Y11" s="2"/>
     </row>
     <row r="12">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="A12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="C12" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="I12" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0.5</v>
+      </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="2"/>
@@ -29960,7 +30536,7 @@
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="E13" s="5"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="2"/>
@@ -43043,4 +43619,342 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="25.43"/>
+    <col customWidth="1" min="3" max="3" width="22.57"/>
+    <col customWidth="1" min="4" max="4" width="21.86"/>
+    <col customWidth="1" min="5" max="5" width="37.71"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3" ht="32.25" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F7" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F8" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="L9" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="3">
+        <v>9.0</v>
+      </c>
+      <c r="C10" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F10" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="I10" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="3">
+        <v>9.0</v>
+      </c>
+      <c r="C11" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F11" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="3"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updating documentation for end of iteration 3
</commit_message>
<xml_diff>
--- a/docs/CS673Team1_weeklyreport.xlsx
+++ b/docs/CS673Team1_weeklyreport.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="162">
   <si>
     <t>week #
  (from date - end date)</t>
@@ -72,51 +72,30 @@
     <t>1 (1/20 - 1/26)</t>
   </si>
   <si>
-    <t>0- started working on tutorial of java Script</t>
+    <t xml:space="preserve"> 0 - research MEAN Stack</t>
   </si>
   <si>
     <t>2 (1/27 - 2/2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0- conitnued  with java Script </t>
-  </si>
-  <si>
-    <t>2 (2/3 - 2/9)</t>
-  </si>
-  <si>
-    <t>0- started learning node.js</t>
-  </si>
-  <si>
-    <t>4 (2/9/ - 2/15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0 - research MEAN Stack</t>
-  </si>
-  <si>
-    <t>5 (2/17 - 2/23)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-3- start project</t>
   </si>
   <si>
     <t>0 - read tutorials on Node.js 
 and MongoDB</t>
   </si>
   <si>
-    <t>0-learning angular js and node.js</t>
+    <t>2 (2/3 - 2/9)</t>
+  </si>
+  <si>
+    <t>0- started working on tutorial of java Script</t>
   </si>
   <si>
     <t>0 - look through sample project
 code</t>
   </si>
   <si>
-    <t xml:space="preserve">2-begin designing db models schema and cloud environment
-3-more coding
-</t>
+    <t>0,2</t>
   </si>
   <si>
-    <t>0,2</t>
+    <t>4 (2/9/ - 2/15)</t>
   </si>
   <si>
     <t>0 - research SCMP and how to
@@ -128,8 +107,14 @@
     <t>2,3</t>
   </si>
   <si>
-    <t>3-adding to existing project code,
- implementing web-socket into backend</t>
+    <t xml:space="preserve">
+3- start project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0- conitnued  with java Script </t>
+  </si>
+  <si>
+    <t>5 (2/17 - 2/23)</t>
   </si>
   <si>
     <t>2 - decide on how the posts  
@@ -137,17 +122,26 @@
 3 - start writing html code for the posts</t>
   </si>
   <si>
+    <t xml:space="preserve">2-begin designing db models schema and cloud environment
+3-more coding
+</t>
+  </si>
+  <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>0- started learning node.js</t>
   </si>
   <si>
     <t>6 (2/24 - 3/2)</t>
   </si>
   <si>
+    <t>3-adding to existing project code,
+ implementing web-socket into backend</t>
+  </si>
+  <si>
     <t>3 - start writing back end
 functionality for wall posts</t>
-  </si>
-  <si>
-    <t>7 (3/3 - 3/9)</t>
   </si>
   <si>
     <t xml:space="preserve">research 
@@ -158,10 +152,23 @@
 </t>
   </si>
   <si>
+    <t>7 (3/3 - 3/9)</t>
+  </si>
+  <si>
+    <t>chat 
+deployment research, async js research, websockket research
+Angular and node JS Security</t>
+  </si>
+  <si>
     <t>3 - add finishing touches to wall
 4 - start testing wall posts to make
 they're working as expected
 6 - get ready for git merge</t>
+  </si>
+  <si>
+    <t>merge
+chat room front end design
+chat front end controller</t>
   </si>
   <si>
     <t>3,2</t>
@@ -170,29 +177,7 @@
     <t>8 (3/10 - 3/16)</t>
   </si>
   <si>
-    <t>3- wokring for about me page using bootstrap
-3.workinf on designing of authorization page.</t>
-  </si>
-  <si>
-    <t>chat 
-deployment research, async js research, websockket research
-Angular and node JS Security</t>
-  </si>
-  <si>
-    <t>2 - start looking into how to add
-comments to a post
-3 - work on defect</t>
-  </si>
-  <si>
-    <t>0- learning animation and dynamic page chnages</t>
-  </si>
-  <si>
-    <t>merge
-chat room front end design
-chat front end controller</t>
-  </si>
-  <si>
-    <t>9 (3/17 - 3/23)</t>
+    <t>0-learning angular js and node.js</t>
   </si>
   <si>
     <t xml:space="preserve">Socket Event handler
@@ -202,28 +187,53 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">1 - Added users stories to backlog 1 - Backlog grooming and iteration planning with team 3 - start initial coding for Comments </t>
+    <t>9 (3/17 - 3/23)</t>
   </si>
   <si>
-    <t>3.designingauthorization page</t>
+    <t>2 - start looking into how to add
+comments to a post
+3 - work on defect</t>
   </si>
   <si>
     <t>10 (3/24 - 3/30)</t>
   </si>
   <si>
-    <t>3 - Add functionality to send a friend Request</t>
-  </si>
-  <si>
-    <t>0-Learning angular js for chat feature</t>
+    <t>3- wokring for about me page using bootstrap
+3.workinf on designing of authorization page.</t>
   </si>
   <si>
     <t>Teaching team about angular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Added users stories to backlog 1 - Backlog grooming and iteration planning with team 3 - start initial coding for Comments </t>
   </si>
   <si>
     <t>11 (3/31 - 4/6)</t>
   </si>
   <si>
     <t>Teaching sub group about anuglar/socketio</t>
+  </si>
+  <si>
+    <t>12 (4/7 - 4/13)</t>
+  </si>
+  <si>
+    <t>0- learning animation and dynamic page chnages</t>
+  </si>
+  <si>
+    <t>3 - Add functionality to send a friend Request</t>
+  </si>
+  <si>
+    <t>0 - Deployment Research
+3 - Preparing some application code for deployment</t>
+  </si>
+  <si>
+    <t>3.designingauthorization page</t>
+  </si>
+  <si>
+    <t>0-Learning angular js for chat feature</t>
+  </si>
+  <si>
+    <t>13 (4/14 - 4/20)</t>
   </si>
   <si>
     <t>3 - add functionality to accept friend request and add friend and deny request 5. Meet to plan for presentation and prepare for demo</t>
@@ -238,27 +248,6 @@
     <t>0 - I began going through MEAN tutorials to understand the API and development environments</t>
   </si>
   <si>
-    <t>2 (1/26/2017 - 2/1/2017)</t>
-  </si>
-  <si>
-    <t>0 - I continued going through tutorials and brought up a webserver on my Windows machine so that I can run the code</t>
-  </si>
-  <si>
-    <t>3 (2/2/2017 - 2/8/2017)</t>
-  </si>
-  <si>
-    <t>0 - Read up on html and javascript</t>
-  </si>
-  <si>
-    <t>3 - began implementing the profile options page in the application</t>
-  </si>
-  <si>
-    <t>4 (2/9/2017 - 2/15/2017)</t>
-  </si>
-  <si>
-    <t>0 - read up on node.js</t>
-  </si>
-  <si>
     <t>0 - Reading tutorials, setting up environment, and doing traning exercises for MEAN technology stack
 0 - Reading Encounter case studies to prepare topics for team meeting
 5 - Discussions with team about course logistics, setting meeting time, etc.</t>
@@ -267,6 +256,12 @@
     <t>0 - Continue learning about MEAN stack
 1 - Come up with some desired app features, reference similar apps, so we can draft requirements
 1 - Start work on SQAP section of SPPP</t>
+  </si>
+  <si>
+    <t>2 (1/26/2017 - 2/1/2017)</t>
+  </si>
+  <si>
+    <t>0 - I continued going through tutorials and brought up a webserver on my Windows machine so that I can run the code</t>
   </si>
   <si>
     <t>0 - Learning about node.js
@@ -287,22 +282,13 @@
 1 - Investigating capabilities of node modules to do OAuth with Facebook/Google</t>
   </si>
   <si>
-    <t>5 (2/16/2017 - 2/22/2017)</t>
-  </si>
-  <si>
     <t>0 - Continue learning about node.js
 1 - Finish Requirements section of SPPP
 1 - Finish SQAP section of SPPP
 2 - Work on design for authentication</t>
   </si>
   <si>
-    <t>3 - worked on implementing profile options page in the application</t>
-  </si>
-  <si>
     <t>4 (2/10 - 2/16)</t>
-  </si>
-  <si>
-    <t>Implement profile options page</t>
   </si>
   <si>
     <t>0 - Learning about express.js
@@ -312,7 +298,7 @@
 5 - Coordinate with team on SPPP and presentation</t>
   </si>
   <si>
-    <t>6 (2/23/2017 - 3/1/2017)</t>
+    <t>3 (2/2/2017 - 2/8/2017)</t>
   </si>
   <si>
     <t>0 - Continue learning about node and express.js
@@ -321,10 +307,7 @@
 3 - Start implementation for authentication</t>
   </si>
   <si>
-    <t>3 - wored on implementing profile options page in the application</t>
-  </si>
-  <si>
-    <t>Finish implementation of profile options page</t>
+    <t>0 - Read up on html and javascript</t>
   </si>
   <si>
     <t>0 - Learning about express.js
@@ -332,23 +315,23 @@
 3 - Implementing Facebook OAuth</t>
   </si>
   <si>
-    <t>7 (3/2/2017 - 3/8/2017)</t>
-  </si>
-  <si>
     <t>0 - Continue learning about express.js
 1 - Create user stories for OAuth with Facebook, Google
 3 - Add unit tests for Authentication modules, give detailed description for team members to follow</t>
   </si>
   <si>
-    <t>3 - Integrated profile feature with development branch</t>
+    <t>3 - began implementing the profile options page in the application</t>
   </si>
   <si>
-    <t>Work on presentation and paper</t>
+    <t>4 (2/9/2017 - 2/15/2017)</t>
   </si>
   <si>
     <t>0 - Learning about express.js
 1 - Requirements analysis for Authentication and Search by email
 3 - Adding unit tests for front-end and back-end authentication modules with commentary for team</t>
+  </si>
+  <si>
+    <t>0 - read up on node.js</t>
   </si>
   <si>
     <t>1 - Add more user stories, meet with team to prioritize
@@ -357,26 +340,14 @@
 4 - Start preparing test plan</t>
   </si>
   <si>
-    <t>5 - Prepared slides for the presentation</t>
-  </si>
-  <si>
     <t>1 - Added users stories to backlog
 3 - Worked with team to merge everyone's work
 4 - Created test plan
 4 - Tested features</t>
   </si>
   <si>
-    <t>8 (3/9/2017 - 3/15/2017)</t>
-  </si>
-  <si>
     <t>3 - Implement Google OAuth
 4 - Finish all testing for iteration 1</t>
-  </si>
-  <si>
-    <t>3 - Reviews integration changes to get profile to work</t>
-  </si>
-  <si>
-    <t>Begin new feature development</t>
   </si>
   <si>
     <t>3 - Added more unit tests
@@ -385,15 +356,9 @@
 4 - Bug fixes</t>
   </si>
   <si>
-    <t>5 - Editted slides and reviewed paper</t>
-  </si>
-  <si>
     <t>1 - Add user stories to backlog
 1 - Backlog grooming and prioritization
 3 - Work on combining profile data and wall posts into single view</t>
-  </si>
-  <si>
-    <t>9 (3/16/2017 - 3/22/2017)</t>
   </si>
   <si>
     <t>1 - Added users stories to backlog
@@ -401,36 +366,18 @@
 3 - Combined the user's profile data and wall posts into a single view</t>
   </si>
   <si>
-    <t>3 - attempted to merge profile info and wall pages</t>
-  </si>
-  <si>
     <t>3 - Allow users to view other users' profiles
 3 - Don't show other users' profiles as editable forms</t>
-  </si>
-  <si>
-    <t>Attempt to get backend to produce other user's profile pages</t>
-  </si>
-  <si>
-    <t>10 (3/23/2017 - 3/29/2017)</t>
   </si>
   <si>
     <t>3 - Allow users to view other users' profile pages
 3 - Add toggle option for making profile info form editable</t>
   </si>
   <si>
-    <t>Bad week.  Didn't have time to do anything so far.</t>
-  </si>
-  <si>
     <t>3 - Don't show other users' profiles as editable forms
 3 - Only show wall posts for the profile you are viewing
 4 - Update test plan and run regression tests
 4 - Collect test results for testing report, include code coverage</t>
-  </si>
-  <si>
-    <t>11 (3/30/2017 - 4/5/2017)</t>
-  </si>
-  <si>
-    <t>0 - Read through documentation regarding route script file</t>
   </si>
   <si>
     <t>3 - Make wall posts specific to a user, a user's wall posts appear only on their profile
@@ -441,6 +388,105 @@
 4 - Tested features</t>
   </si>
   <si>
+    <t>3 - Add logout functionality
+3 - Show user information on wall posts</t>
+  </si>
+  <si>
+    <t>5 (2/16/2017 - 2/22/2017)</t>
+  </si>
+  <si>
+    <t>3 - Added logout functionality
+3 - Started work on showing user information on wall posts</t>
+  </si>
+  <si>
+    <t>3 - Show user information on wall posts
+3 - Show user information on chat messages</t>
+  </si>
+  <si>
+    <t>3 - worked on implementing profile options page in the application</t>
+  </si>
+  <si>
+    <t>Implement profile options page</t>
+  </si>
+  <si>
+    <t>3 - Finished work on showing user information on wall posts
+3 - Worked on new login page layout
+3 - Started work on showing user information on chat messages</t>
+  </si>
+  <si>
+    <t>3 - Show user infomation on chat messages
+3 - Show search results
+3 - Fix missing timestamps on wall messages
+3 - Fix wall post comments</t>
+  </si>
+  <si>
+    <t>14 (4/21 - 4/27)</t>
+  </si>
+  <si>
+    <t>6 (2/23/2017 - 3/1/2017)</t>
+  </si>
+  <si>
+    <t>3 - wored on implementing profile options page in the application</t>
+  </si>
+  <si>
+    <t>3 - Integrated picture/name with comments, chate messages, search results
+3 - Improved user experience in terms of transition from login to profile and UI design
+3 - Lots of stablization and configuration to make the app deployable in locations other than on local system
+4 - Lots of testing on deployed product</t>
+  </si>
+  <si>
+    <t>6 - Sleep
+6 - Study</t>
+  </si>
+  <si>
+    <t>Finish implementation of profile options page</t>
+  </si>
+  <si>
+    <t>7 (3/2/2017 - 3/8/2017)</t>
+  </si>
+  <si>
+    <t>3 - Integrated profile feature with development branch</t>
+  </si>
+  <si>
+    <t>Work on presentation and paper</t>
+  </si>
+  <si>
+    <t>5 - Prepared slides for the presentation</t>
+  </si>
+  <si>
+    <t>8 (3/9/2017 - 3/15/2017)</t>
+  </si>
+  <si>
+    <t>3 - Reviews integration changes to get profile to work</t>
+  </si>
+  <si>
+    <t>Begin new feature development</t>
+  </si>
+  <si>
+    <t>5 - Editted slides and reviewed paper</t>
+  </si>
+  <si>
+    <t>9 (3/16/2017 - 3/22/2017)</t>
+  </si>
+  <si>
+    <t>3 - attempted to merge profile info and wall pages</t>
+  </si>
+  <si>
+    <t>Attempt to get backend to produce other user's profile pages</t>
+  </si>
+  <si>
+    <t>10 (3/23/2017 - 3/29/2017)</t>
+  </si>
+  <si>
+    <t>Bad week.  Didn't have time to do anything so far.</t>
+  </si>
+  <si>
+    <t>11 (3/30/2017 - 4/5/2017)</t>
+  </si>
+  <si>
+    <t>0 - Read through documentation regarding route script file</t>
+  </si>
+  <si>
     <t>3 - modified routing code to support passing of profile data by performing an http get on api/profile/username</t>
   </si>
   <si>
@@ -448,6 +494,33 @@
   </si>
   <si>
     <t>12 (4/6/2017 - 4/12/2017)</t>
+  </si>
+  <si>
+    <t>5 - Worked on slides</t>
+  </si>
+  <si>
+    <t>Work on search feature</t>
+  </si>
+  <si>
+    <t>13 (4/13/2017 - 4/19/2017)</t>
+  </si>
+  <si>
+    <t>3 - Started working on search page.  Didn't get it to work</t>
+  </si>
+  <si>
+    <t>Finish search page</t>
+  </si>
+  <si>
+    <t>14 (4/20/2017 - 4/26/2017)</t>
+  </si>
+  <si>
+    <t>3 - Fixed search page so you can search database from web interface</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>0 - Read documentation on using regular expressions to query mongo database</t>
   </si>
   <si>
     <t>0 - Learning more about the MEAN stack via tutorials.
@@ -502,6 +575,30 @@
 6 - started the slides for Iteration #2 demo</t>
   </si>
   <si>
+    <t>3 - worked on picture upload functionality to stay and refresh the page after upload instead of redirecting to another page
+3 - worked on deleting a picture from a user's picture gallery
+5 - assigned tasks within subgroup
+3 - working on user's picture gallery - ability to only see your pictures</t>
+  </si>
+  <si>
+    <t>11 (4/14 - 4/20)</t>
+  </si>
+  <si>
+    <t>4 - tested Ravi's branch of assigning a picture to a profile
+3 - merged Ravi's branch into the development branch
+3 - working on user's picture gallery - ability to only see your pictures</t>
+  </si>
+  <si>
+    <t>11 (4/21 - 4/27)</t>
+  </si>
+  <si>
+    <t>3 - work on limiting file uploads to only image files
+3 - work on limiting file sizes when uploading images
+3 - gracefully show an error when no file selected, and the submit button is pressed
+3 - working on user's picture gallery - ability to only see your pictures
+5 - working on slides for final demo</t>
+  </si>
+  <si>
     <t>0- Learning MEAN basics</t>
   </si>
   <si>
@@ -531,12 +628,24 @@
     <t>2- Chat design
 3- Implementing chat scroll feature</t>
   </si>
+  <si>
+    <t>2- Designed the model and controller for the
+    profile picture</t>
+  </si>
+  <si>
+    <t>3- Implementing the set-profile picture</t>
+  </si>
+  <si>
+    <t>2-Designed the comments section
+3-Implemented the comment section
+3-Implemented the posting feature on the wall</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -548,6 +657,11 @@
     <font/>
     <font>
       <color rgb="FFFF0000"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <color rgb="FF000000"/>
@@ -582,7 +696,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -594,25 +708,28 @@
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -744,7 +861,7 @@
         <v>1.0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F2" s="3">
         <v>2.0</v>
@@ -779,7 +896,7 @@
         <v>1.0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="F3" s="3">
         <v>2.0</v>
@@ -815,7 +932,7 @@
         <v>1.0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F4" s="3">
         <v>2.0</v>
@@ -842,7 +959,7 @@
     </row>
     <row r="5" ht="21.0" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -871,7 +988,7 @@
     </row>
     <row r="6" ht="34.5" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B6" s="3">
         <v>5.0</v>
@@ -883,7 +1000,7 @@
         <v>1.0</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="F6" s="3">
         <v>3.0</v>
@@ -901,7 +1018,7 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" s="3">
         <v>4.0</v>
@@ -913,7 +1030,7 @@
         <v>1.0</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F7" s="3">
         <v>2.0</v>
@@ -943,7 +1060,7 @@
         <v>2.0</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G8" s="3">
         <v>1.0</v>
@@ -961,7 +1078,7 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3">
         <v>4.0</v>
@@ -973,7 +1090,7 @@
         <v>0.5</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="I9" s="3">
         <v>4.5</v>
@@ -984,7 +1101,7 @@
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="3">
         <v>4.0</v>
@@ -996,7 +1113,7 @@
         <v>3.0</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F10" s="3">
         <v>3.0</v>
@@ -1023,7 +1140,7 @@
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B11" s="3">
         <v>4.0</v>
@@ -15228,7 +15345,7 @@
         <v>1.0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F2" s="3">
         <v>5.0</v>
@@ -15248,7 +15365,7 @@
         <v>2.0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F3" s="3"/>
       <c r="I3" s="3">
@@ -15269,7 +15386,7 @@
         <v>2.0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F4" s="3"/>
       <c r="H4" s="3">
@@ -15281,7 +15398,7 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3">
         <v>8.0</v>
@@ -15293,7 +15410,7 @@
         <v>2.0</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F5" s="3"/>
       <c r="I5" s="3">
@@ -15302,7 +15419,7 @@
     </row>
     <row r="6" ht="58.5" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B6" s="3">
         <v>7.0</v>
@@ -15314,12 +15431,12 @@
         <v>1.0</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" ht="39.0" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" s="3">
         <v>8.0</v>
@@ -15331,7 +15448,7 @@
         <v>1.0</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" ht="36.0" customHeight="1">
@@ -15348,12 +15465,12 @@
         <v>2.0</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" ht="29.25" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3">
         <v>9.0</v>
@@ -15365,12 +15482,12 @@
         <v>1.0</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="3">
         <v>8.0</v>
@@ -15382,12 +15499,12 @@
         <v>1.0</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B11" s="3">
         <v>7.0</v>
@@ -15399,12 +15516,12 @@
         <v>3.0</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B12" s="3">
         <v>6.0</v>
@@ -15416,8 +15533,31 @@
         <v>3.0</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="C13" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>55</v>
       </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -15493,7 +15633,7 @@
         <v>1.0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F2" s="3">
         <v>6.0</v>
@@ -15516,7 +15656,7 @@
         <v>2.0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F3" s="3">
         <v>5.0</v>
@@ -15539,13 +15679,13 @@
         <v>2.0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F4" s="3">
         <v>5.0</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="N4" s="3">
         <v>8.0</v>
@@ -15553,7 +15693,7 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3">
         <v>6.0</v>
@@ -15562,7 +15702,7 @@
         <v>2.0</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F5" s="3">
         <v>2.0</v>
@@ -15571,7 +15711,7 @@
         <v>4.0</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="N5" s="3">
         <v>10.0</v>
@@ -15579,7 +15719,7 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B6" s="3">
         <v>7.0</v>
@@ -15588,10 +15728,10 @@
         <v>1.0</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H6" s="3">
         <v>1.0</v>
@@ -15608,7 +15748,7 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" s="3">
         <v>9.0</v>
@@ -15617,7 +15757,7 @@
         <v>1.0</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I7" s="3">
         <v>8.0</v>
@@ -15652,7 +15792,7 @@
         <v>2.0</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N8" s="3">
         <v>8.0</v>
@@ -15660,7 +15800,7 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3">
         <v>4.0</v>
@@ -15669,7 +15809,7 @@
         <v>1.0</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H9" s="3">
         <v>2.0</v>
@@ -15683,7 +15823,7 @@
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="3">
         <v>5.0</v>
@@ -15695,7 +15835,7 @@
         <v>3.0</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G10" s="3">
         <v>3.0</v>
@@ -15713,7 +15853,7 @@
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B11" s="3">
         <v>7.0</v>
@@ -15725,13 +15865,13 @@
         <v>0.0</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="I11" s="3">
         <v>7.0</v>
       </c>
       <c r="K11" s="3"/>
-      <c r="M11" s="5">
+      <c r="M11" s="6">
         <v>3.0</v>
       </c>
       <c r="N11" s="3">
@@ -15740,7 +15880,7 @@
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B12" s="3">
         <v>9.0</v>
@@ -15752,7 +15892,7 @@
         <v>3.0</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I12" s="3">
         <v>6.0</v>
@@ -15761,7 +15901,7 @@
         <v>3.0</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="N12" s="3">
         <v>8.0</v>
@@ -15848,7 +15988,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B2" s="3">
         <v>6.0</v>
@@ -15860,7 +16000,7 @@
         <v>1.0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F2" s="3">
         <v>5.0</v>
@@ -15899,7 +16039,7 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B3" s="3">
         <v>5.0</v>
@@ -15911,7 +16051,7 @@
         <v>1.0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F3" s="3">
         <v>4.0</v>
@@ -15931,7 +16071,7 @@
       <c r="K3" s="3">
         <v>0.0</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="7">
         <v>0.0</v>
       </c>
       <c r="M3" s="3"/>
@@ -15952,7 +16092,7 @@
     </row>
     <row r="4" ht="16.5" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="B4" s="3">
         <v>8.0</v>
@@ -15964,7 +16104,7 @@
         <v>1.0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="F4" s="3">
         <v>1.0</v>
@@ -16009,7 +16149,7 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -16034,7 +16174,7 @@
     </row>
     <row r="6" ht="4.5" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="B6" s="3">
         <v>8.0</v>
@@ -16046,7 +16186,7 @@
         <v>1.0</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="F6" s="3">
         <v>1.0</v>
@@ -16086,22 +16226,22 @@
       <c r="Y6" s="2"/>
     </row>
     <row r="7" ht="19.5" customHeight="1">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="8">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="9">
         <v>8.0</v>
       </c>
       <c r="O7" s="2"/>
@@ -16118,7 +16258,7 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="B8" s="3">
         <v>8.0</v>
@@ -16130,7 +16270,7 @@
         <v>1.0</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="F8" s="3">
         <v>0.0</v>
@@ -16154,7 +16294,7 @@
         <v>0.0</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="N8" s="3">
         <v>8.0</v>
@@ -16173,7 +16313,7 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="B9" s="3">
         <v>5.0</v>
@@ -16185,7 +16325,7 @@
         <v>1.0</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="F9" s="3">
         <v>0.0</v>
@@ -16209,7 +16349,7 @@
         <v>0.0</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="N9" s="3">
         <v>8.0</v>
@@ -16228,7 +16368,7 @@
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="B10" s="3">
         <v>12.0</v>
@@ -16240,7 +16380,7 @@
         <v>4.0</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="F10" s="3">
         <v>1.0</v>
@@ -16264,7 +16404,7 @@
         <v>0.0</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="N10" s="3">
         <v>8.0</v>
@@ -16287,7 +16427,7 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -16311,7 +16451,7 @@
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="B12" s="3">
         <v>9.0</v>
@@ -16323,7 +16463,7 @@
         <v>4.0</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="F12" s="3">
         <v>0.0</v>
@@ -16347,7 +16487,7 @@
         <v>0.0</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="N12" s="3">
         <v>8.0</v>
@@ -16366,7 +16506,7 @@
     </row>
     <row r="13">
       <c r="E13" s="3" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -16389,7 +16529,7 @@
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B14" s="3">
         <v>5.0</v>
@@ -16401,7 +16541,7 @@
         <v>1.0</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="F14" s="3">
         <v>0.0</v>
@@ -16425,7 +16565,7 @@
         <v>0.0</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="N14" s="3">
         <v>8.0</v>
@@ -16444,7 +16584,7 @@
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="B15" s="3">
         <v>1.0</v>
@@ -16456,7 +16596,7 @@
         <v>1.0</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="F15" s="3">
         <v>0.0</v>
@@ -16480,7 +16620,7 @@
         <v>0.0</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="N15" s="3">
         <v>8.0</v>
@@ -16499,7 +16639,7 @@
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="B16" s="3">
         <v>18.0</v>
@@ -16511,7 +16651,7 @@
         <v>2.0</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="F16" s="3">
         <v>2.0</v>
@@ -16531,7 +16671,7 @@
       <c r="K16" s="3">
         <v>2.0</v>
       </c>
-      <c r="L16" s="6">
+      <c r="L16" s="7">
         <v>0.0</v>
       </c>
       <c r="M16" s="3"/>
@@ -16554,7 +16694,7 @@
       <c r="A17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -16578,7 +16718,7 @@
       <c r="A18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
@@ -16594,13 +16734,44 @@
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+        <v>124</v>
+      </c>
+      <c r="B19" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="C19" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I19" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="K19" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="L19" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
@@ -16630,7 +16801,48 @@
       <c r="Y20" s="2"/>
     </row>
     <row r="21">
-      <c r="A21" s="3"/>
+      <c r="A21" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B21" s="3">
+        <v>9.0</v>
+      </c>
+      <c r="C21" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I21" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="K21" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="L21" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="N21" s="3">
+        <v>8.0</v>
+      </c>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
@@ -16669,15 +16881,48 @@
       <c r="Y22" s="2"/>
     </row>
     <row r="23">
-      <c r="A23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
+      <c r="A23" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" s="3">
+        <v>14.0</v>
+      </c>
+      <c r="C23" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F23" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I23" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="J23" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="K23" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="L23" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="N23" s="3">
+        <v>0.0</v>
+      </c>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
@@ -16693,7 +16938,9 @@
     <row r="24">
       <c r="A24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="E24" s="3" t="s">
+        <v>133</v>
+      </c>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
@@ -29688,7 +29935,7 @@
         <v>1.0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F2" s="3">
         <v>4.5</v>
@@ -29697,7 +29944,7 @@
         <v>0.5</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="N2" s="3">
         <v>8.0</v>
@@ -29717,7 +29964,7 @@
         <v>2.0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F3" s="3">
         <v>2.0</v>
@@ -29726,7 +29973,7 @@
         <v>1.0</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N3" s="3">
         <v>6.0</v>
@@ -29734,7 +29981,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B4" s="3">
         <v>5.0</v>
@@ -29746,7 +29993,7 @@
         <v>1.0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F4" s="3">
         <v>3.0</v>
@@ -29755,7 +30002,7 @@
         <v>1.0</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="N4" s="3">
         <v>6.0</v>
@@ -29763,7 +30010,7 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B5" s="3">
         <v>8.0</v>
@@ -29775,7 +30022,7 @@
         <v>1.0</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F5" s="3">
         <v>3.0</v>
@@ -29787,7 +30034,7 @@
         <v>1.0</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="N5" s="3">
         <v>6.0</v>
@@ -29795,7 +30042,7 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B6" s="3">
         <v>8.0</v>
@@ -29807,7 +30054,7 @@
         <v>1.0</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F6" s="3">
         <v>3.0</v>
@@ -29819,7 +30066,7 @@
         <v>3.0</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="N6" s="3">
         <v>6.0</v>
@@ -29827,7 +30074,7 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" s="3">
         <v>9.0</v>
@@ -29839,7 +30086,7 @@
         <v>1.0</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F7" s="3">
         <v>2.0</v>
@@ -29851,7 +30098,7 @@
         <v>3.0</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="N7" s="3">
         <v>8.0</v>
@@ -29871,7 +30118,7 @@
         <v>2.0</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="G8" s="3">
         <v>1.0</v>
@@ -29883,7 +30130,7 @@
         <v>3.0</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="N8" s="3">
         <v>4.0</v>
@@ -29891,7 +30138,7 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3">
         <v>7.0</v>
@@ -29903,7 +30150,7 @@
         <v>1.5</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="I9" s="3">
         <v>4.5</v>
@@ -29912,7 +30159,7 @@
         <v>1.0</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="N9" s="3">
         <v>5.0</v>
@@ -29920,7 +30167,7 @@
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="3">
         <v>6.5</v>
@@ -29932,7 +30179,7 @@
         <v>3.0</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="G10" s="3">
         <v>3.0</v>
@@ -29944,7 +30191,7 @@
         <v>0.5</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="N10" s="3">
         <v>5.0</v>
@@ -29952,7 +30199,7 @@
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B11" s="3">
         <v>4.5</v>
@@ -29964,7 +30211,7 @@
         <v>0.0</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="I11" s="3">
         <v>4.0</v>
@@ -29972,8 +30219,8 @@
       <c r="K11" s="3">
         <v>0.5</v>
       </c>
-      <c r="M11" s="5" t="s">
-        <v>107</v>
+      <c r="M11" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="N11" s="3">
         <v>8.0</v>
@@ -29981,7 +30228,7 @@
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B12" s="3">
         <v>14.5</v>
@@ -29993,7 +30240,7 @@
         <v>1.0</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="I12" s="3">
         <v>10.0</v>
@@ -30003,6 +30250,96 @@
       </c>
       <c r="K12" s="3">
         <v>1.0</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="N12" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="C13" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I13" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="K13" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="N13" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="C14" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="I14" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="K14" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="N14" s="3">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="3">
+        <v>22.0</v>
+      </c>
+      <c r="C15" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I15" s="3">
+        <v>15.0</v>
+      </c>
+      <c r="J15" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -30098,7 +30435,7 @@
         <v>1.0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="F2" s="3">
         <v>6.0</v>
@@ -30137,7 +30474,7 @@
         <v>2.5</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="F3" s="3">
         <v>2.0</v>
@@ -30164,7 +30501,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B4" s="3">
         <v>6.0</v>
@@ -30176,7 +30513,7 @@
         <v>1.0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="F4" s="3">
         <v>4.0</v>
@@ -30204,7 +30541,7 @@
     </row>
     <row r="5" ht="27.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="B5" s="3">
         <v>2.5</v>
@@ -30214,7 +30551,7 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3">
@@ -30242,7 +30579,7 @@
     </row>
     <row r="6" ht="34.5" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B6" s="3">
         <v>6.0</v>
@@ -30252,7 +30589,7 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="F6" s="3">
         <v>3.0</v>
@@ -30281,7 +30618,7 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" s="3">
         <v>15.0</v>
@@ -30293,7 +30630,7 @@
         <v>2.0</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="F7" s="3">
         <v>4.0</v>
@@ -30322,7 +30659,7 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="B8" s="3">
         <v>8.0</v>
@@ -30334,7 +30671,7 @@
         <v>6.0</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -30362,7 +30699,7 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3">
         <v>16.0</v>
@@ -30374,7 +30711,7 @@
         <v>4.0</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="F9" s="3">
         <v>1.0</v>
@@ -30402,7 +30739,7 @@
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="3">
         <v>8.0</v>
@@ -30414,7 +30751,7 @@
         <v>1.0</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="F10" s="3">
         <v>1.0</v>
@@ -30449,7 +30786,7 @@
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B11" s="3">
         <v>6.5</v>
@@ -30461,7 +30798,7 @@
         <v>0.5</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -30491,7 +30828,7 @@
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B12" s="3">
         <v>11.0</v>
@@ -30503,7 +30840,7 @@
         <v>1.0</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -30532,11 +30869,28 @@
       <c r="Y12" s="2"/>
     </row>
     <row r="13">
-      <c r="A13" s="3"/>
+      <c r="A13" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="5"/>
+      <c r="C13" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="I13" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K13" s="3">
+        <v>0.5</v>
+      </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="2"/>
@@ -30552,17 +30906,31 @@
       <c r="Y13" s="2"/>
     </row>
     <row r="14">
-      <c r="A14" s="3"/>
+      <c r="A14" s="3" t="s">
+        <v>147</v>
+      </c>
       <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="C14" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>148</v>
+      </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="I14" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K14" s="3">
+        <v>0.5</v>
+      </c>
       <c r="L14" s="4"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
@@ -30579,9 +30947,13 @@
       <c r="Y14" s="2"/>
     </row>
     <row r="15">
-      <c r="A15" s="3"/>
+      <c r="A15" s="3" t="s">
+        <v>149</v>
+      </c>
       <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>150</v>
+      </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -43631,7 +44003,7 @@
     <col customWidth="1" min="2" max="2" width="25.43"/>
     <col customWidth="1" min="3" max="3" width="22.57"/>
     <col customWidth="1" min="4" max="4" width="21.86"/>
-    <col customWidth="1" min="5" max="5" width="37.71"/>
+    <col customWidth="1" min="5" max="5" width="39.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -43694,7 +44066,7 @@
         <v>1.0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="F2" s="3">
         <v>2.0</v>
@@ -43713,8 +44085,8 @@
       <c r="D3" s="3">
         <v>1.0</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>127</v>
+      <c r="E3" s="12" t="s">
+        <v>152</v>
       </c>
       <c r="F3" s="3">
         <v>1.0</v>
@@ -43722,121 +44094,121 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>128</v>
+        <v>69</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>128</v>
+        <v>136</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>128</v>
+        <v>27</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" s="3">
         <v>7.0</v>
@@ -43848,7 +44220,7 @@
         <v>2.0</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
       <c r="F7" s="3">
         <v>3.0</v>
@@ -43859,7 +44231,7 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="B8" s="3">
         <v>11.0</v>
@@ -43871,7 +44243,7 @@
         <v>1.0</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="F8" s="3">
         <v>4.0</v>
@@ -43883,7 +44255,7 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3">
         <v>6.0</v>
@@ -43895,7 +44267,7 @@
         <v>1.0</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="F9" s="3">
         <v>2.0</v>
@@ -43907,7 +44279,7 @@
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="3">
         <v>9.0</v>
@@ -43919,7 +44291,7 @@
         <v>3.0</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="F10" s="3">
         <v>2.0</v>
@@ -43930,7 +44302,7 @@
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B11" s="3">
         <v>9.0</v>
@@ -43942,7 +44314,7 @@
         <v>3.0</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
       <c r="F11" s="3">
         <v>2.0</v>
@@ -43952,7 +44324,74 @@
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="3"/>
+      <c r="A12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="H12" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="I13" s="3">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="C15" s="3">
+        <v>9.0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H15" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="I15" s="3">
+        <v>7.0</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>